<commit_message>
updated data other small changes
</commit_message>
<xml_diff>
--- a/data/real_gdp_US_2022Q4.xlsx
+++ b/data/real_gdp_US_2022Q4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_teaching\_current.teaching\_SU.TSEF\lectures\code-TSEF\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732370F0-5B96-4DBB-A54C-2E03B339EA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E8B9FD-0E60-4D2D-ADB0-292976A9D898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1916" yWindow="1916" windowWidth="14267" windowHeight="24598" xr2:uid="{27CEEFD2-010A-4B54-892D-96BB7408CBE8}"/>
+    <workbookView xWindow="766" yWindow="766" windowWidth="14268" windowHeight="24599" xr2:uid="{27CEEFD2-010A-4B54-892D-96BB7408CBE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
udpate to US gdp data
</commit_message>
<xml_diff>
--- a/data/real_gdp_US_2022Q4.xlsx
+++ b/data/real_gdp_US_2022Q4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_teaching\_current.teaching\_SU.TSEF\lectures\code-TSEF\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_teaching\_current.teaching\_SU.TSEF\code-TSEF\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E8B9FD-0E60-4D2D-ADB0-292976A9D898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CBB80B-A4E3-4320-BEF6-B31880BE92C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="766" yWindow="766" windowWidth="14268" windowHeight="24599" xr2:uid="{27CEEFD2-010A-4B54-892D-96BB7408CBE8}"/>
+    <workbookView xWindow="3792" yWindow="3792" windowWidth="14267" windowHeight="24598" xr2:uid="{27CEEFD2-010A-4B54-892D-96BB7408CBE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="311">
   <si>
     <t>dates</t>
   </si>
@@ -958,6 +958,15 @@
   </si>
   <si>
     <t>01-Jan-2023</t>
+  </si>
+  <si>
+    <t>01-Apr-2023</t>
+  </si>
+  <si>
+    <t>01-Jul-2023</t>
+  </si>
+  <si>
+    <t>01-Oct-2023</t>
   </si>
 </sst>
 </file>
@@ -1310,10 +1319,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A5801BB-9EED-48AD-B5EC-B6A1032E6771}">
-  <dimension ref="A1:C306"/>
+  <dimension ref="A1:C309"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C305"/>
+      <selection activeCell="B2" sqref="B2:C309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.8" x14ac:dyDescent="0.45"/>
@@ -1334,7 +1343,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>2034.45</v>
+        <v>2182.681</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1345,7 +1354,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>2029.0239999999999</v>
+        <v>2176.8919999999998</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1356,7 +1365,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>2024.8340000000001</v>
+        <v>2172.4319999999998</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1367,7 +1376,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>2056.5079999999998</v>
+        <v>2206.4520000000002</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1378,7 +1387,7 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>2087.442</v>
+        <v>2239.6819999999998</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1389,7 +1398,7 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>2121.8989999999999</v>
+        <v>2276.69</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1400,7 +1409,7 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>2134.056</v>
+        <v>2289.77</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1411,7 +1420,7 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>2136.44</v>
+        <v>2292.364</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1422,7 +1431,7 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>2107.0010000000002</v>
+        <v>2260.8069999999998</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1433,7 +1442,7 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>2099.8139999999999</v>
+        <v>2253.1280000000002</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1444,7 +1453,7 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>2121.4929999999999</v>
+        <v>2276.424</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1455,7 +1464,7 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>2103.6880000000001</v>
+        <v>2257.3519999999999</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1466,7 +1475,7 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>2186.3649999999998</v>
+        <v>2346.1039999999998</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1477,7 +1486,7 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>2253.0450000000001</v>
+        <v>2417.6819999999998</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1488,7 +1497,7 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>2340.1120000000001</v>
+        <v>2511.127</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1499,7 +1508,7 @@
         <v>18</v>
       </c>
       <c r="B17">
-        <v>2384.92</v>
+        <v>2559.2139999999999</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1510,7 +1519,7 @@
         <v>19</v>
       </c>
       <c r="B18">
-        <v>2417.3110000000001</v>
+        <v>2593.9670000000001</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1521,7 +1530,7 @@
         <v>20</v>
       </c>
       <c r="B19">
-        <v>2459.1959999999999</v>
+        <v>2638.8980000000001</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1532,7 +1541,7 @@
         <v>21</v>
       </c>
       <c r="B20">
-        <v>2509.88</v>
+        <v>2693.259</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1543,7 +1552,7 @@
         <v>22</v>
       </c>
       <c r="B21">
-        <v>2515.4079999999999</v>
+        <v>2699.1559999999999</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1554,7 +1563,7 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <v>2542.2860000000001</v>
+        <v>2727.9540000000002</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1565,7 +1574,7 @@
         <v>24</v>
       </c>
       <c r="B23">
-        <v>2547.7620000000002</v>
+        <v>2733.8</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1576,7 +1585,7 @@
         <v>25</v>
       </c>
       <c r="B24">
-        <v>2566.1529999999998</v>
+        <v>2753.5169999999998</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1587,7 +1596,7 @@
         <v>26</v>
       </c>
       <c r="B25">
-        <v>2650.431</v>
+        <v>2843.9409999999998</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -1598,7 +1607,7 @@
         <v>27</v>
       </c>
       <c r="B26">
-        <v>2699.6990000000001</v>
+        <v>2896.8110000000001</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -1609,7 +1618,7 @@
         <v>28</v>
       </c>
       <c r="B27">
-        <v>2720.5659999999998</v>
+        <v>2919.2060000000001</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1620,7 +1629,7 @@
         <v>29</v>
       </c>
       <c r="B28">
-        <v>2705.2579999999998</v>
+        <v>2902.7849999999999</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1631,7 +1640,7 @@
         <v>30</v>
       </c>
       <c r="B29">
-        <v>2664.3020000000001</v>
+        <v>2858.8449999999998</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1642,7 +1651,7 @@
         <v>31</v>
       </c>
       <c r="B30">
-        <v>2651.5659999999998</v>
+        <v>2845.192</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1653,7 +1662,7 @@
         <v>32</v>
       </c>
       <c r="B31">
-        <v>2654.4560000000001</v>
+        <v>2848.3049999999998</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1664,7 +1673,7 @@
         <v>33</v>
       </c>
       <c r="B32">
-        <v>2684.4340000000002</v>
+        <v>2880.482</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1675,7 +1684,7 @@
         <v>34</v>
       </c>
       <c r="B33">
-        <v>2736.96</v>
+        <v>2936.8519999999999</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -1686,7 +1695,7 @@
         <v>35</v>
       </c>
       <c r="B34">
-        <v>2815.134</v>
+        <v>3020.7460000000001</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -1697,7 +1706,7 @@
         <v>36</v>
       </c>
       <c r="B35">
-        <v>2860.942</v>
+        <v>3069.91</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1708,7 +1717,7 @@
         <v>37</v>
       </c>
       <c r="B36">
-        <v>2899.578</v>
+        <v>3111.3789999999999</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1719,7 +1728,7 @@
         <v>38</v>
       </c>
       <c r="B37">
-        <v>2916.9850000000001</v>
+        <v>3130.0680000000002</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1730,7 +1739,7 @@
         <v>39</v>
       </c>
       <c r="B38">
-        <v>2905.6559999999999</v>
+        <v>3117.922</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1741,7 +1750,7 @@
         <v>40</v>
       </c>
       <c r="B39">
-        <v>2929.6660000000002</v>
+        <v>3143.694</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1752,7 +1761,7 @@
         <v>41</v>
       </c>
       <c r="B40">
-        <v>2927.0340000000001</v>
+        <v>3140.8739999999998</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1763,7 +1772,7 @@
         <v>42</v>
       </c>
       <c r="B41">
-        <v>2975.2089999999998</v>
+        <v>3192.57</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1774,7 +1783,7 @@
         <v>43</v>
       </c>
       <c r="B42">
-        <v>2994.259</v>
+        <v>3213.011</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -1785,7 +1794,7 @@
         <v>44</v>
       </c>
       <c r="B43">
-        <v>2987.6990000000001</v>
+        <v>3205.97</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -1796,7 +1805,7 @@
         <v>45</v>
       </c>
       <c r="B44">
-        <v>3016.9789999999998</v>
+        <v>3237.386</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -1807,7 +1816,7 @@
         <v>46</v>
       </c>
       <c r="B45">
-        <v>2985.7750000000001</v>
+        <v>3203.8939999999998</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -1818,7 +1827,7 @@
         <v>47</v>
       </c>
       <c r="B46">
-        <v>2908.2809999999999</v>
+        <v>3120.7240000000002</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -1829,7 +1838,7 @@
         <v>48</v>
       </c>
       <c r="B47">
-        <v>2927.395</v>
+        <v>3141.2240000000002</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -1840,7 +1849,7 @@
         <v>49</v>
       </c>
       <c r="B48">
-        <v>2995.1120000000001</v>
+        <v>3213.884</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -1851,7 +1860,7 @@
         <v>50</v>
       </c>
       <c r="B49">
-        <v>3065.1410000000001</v>
+        <v>3289.0320000000002</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -1862,7 +1871,7 @@
         <v>51</v>
       </c>
       <c r="B50">
-        <v>3123.9780000000001</v>
+        <v>3352.1289999999999</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -1873,7 +1882,7 @@
         <v>52</v>
       </c>
       <c r="B51">
-        <v>3194.4290000000001</v>
+        <v>3427.6669999999999</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -1884,7 +1893,7 @@
         <v>53</v>
       </c>
       <c r="B52">
-        <v>3196.683</v>
+        <v>3430.0569999999998</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -1895,7 +1904,7 @@
         <v>54</v>
       </c>
       <c r="B53">
-        <v>3205.79</v>
+        <v>3439.8319999999999</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -1906,7 +1915,7 @@
         <v>55</v>
       </c>
       <c r="B54">
-        <v>3277.8470000000002</v>
+        <v>3517.181</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -1917,7 +1926,7 @@
         <v>56</v>
       </c>
       <c r="B55">
-        <v>3260.1770000000001</v>
+        <v>3498.2460000000001</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -1928,7 +1937,7 @@
         <v>57</v>
       </c>
       <c r="B56">
-        <v>3276.1329999999998</v>
+        <v>3515.3850000000002</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -1939,7 +1948,7 @@
         <v>58</v>
       </c>
       <c r="B57">
-        <v>3234.087</v>
+        <v>3470.2779999999998</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -1950,7 +1959,7 @@
         <v>59</v>
       </c>
       <c r="B58">
-        <v>3255.9140000000002</v>
+        <v>3493.703</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -1961,7 +1970,7 @@
         <v>60</v>
       </c>
       <c r="B59">
-        <v>3311.181</v>
+        <v>3553.0210000000002</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -1972,7 +1981,7 @@
         <v>61</v>
       </c>
       <c r="B60">
-        <v>3374.7420000000002</v>
+        <v>3621.252</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -1983,7 +1992,7 @@
         <v>62</v>
       </c>
       <c r="B61">
-        <v>3440.924</v>
+        <v>3692.2890000000002</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1994,7 +2003,7 @@
         <v>63</v>
       </c>
       <c r="B62">
-        <v>3502.2979999999998</v>
+        <v>3758.1469999999999</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -2005,7 +2014,7 @@
         <v>64</v>
       </c>
       <c r="B63">
-        <v>3533.9470000000001</v>
+        <v>3792.1489999999999</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -2016,7 +2025,7 @@
         <v>65</v>
       </c>
       <c r="B64">
-        <v>3577.3620000000001</v>
+        <v>3838.7759999999998</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -2027,7 +2036,7 @@
         <v>66</v>
       </c>
       <c r="B65">
-        <v>3589.1280000000002</v>
+        <v>3851.4209999999998</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -2038,7 +2047,7 @@
         <v>67</v>
       </c>
       <c r="B66">
-        <v>3628.306</v>
+        <v>3893.482</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -2049,7 +2058,7 @@
         <v>68</v>
       </c>
       <c r="B67">
-        <v>3669.02</v>
+        <v>3937.183</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -2060,7 +2069,7 @@
         <v>69</v>
       </c>
       <c r="B68">
-        <v>3749.681</v>
+        <v>4023.7550000000001</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -2071,7 +2080,7 @@
         <v>70</v>
       </c>
       <c r="B69">
-        <v>3774.2640000000001</v>
+        <v>4050.1469999999999</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -2082,7 +2091,7 @@
         <v>71</v>
       </c>
       <c r="B70">
-        <v>3853.835</v>
+        <v>4135.5529999999999</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -2093,7 +2102,7 @@
         <v>72</v>
       </c>
       <c r="B71">
-        <v>3895.7930000000001</v>
+        <v>4180.5919999999996</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -2104,7 +2113,7 @@
         <v>73</v>
       </c>
       <c r="B72">
-        <v>3956.6570000000002</v>
+        <v>4245.9179999999997</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -2115,7 +2124,7 @@
         <v>74</v>
       </c>
       <c r="B73">
-        <v>3968.8780000000002</v>
+        <v>4259.0460000000003</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -2126,7 +2135,7 @@
         <v>75</v>
       </c>
       <c r="B74">
-        <v>4064.915</v>
+        <v>4362.1109999999999</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -2137,7 +2146,7 @@
         <v>76</v>
       </c>
       <c r="B75">
-        <v>4116.2669999999998</v>
+        <v>4417.2250000000004</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -2148,7 +2157,7 @@
         <v>77</v>
       </c>
       <c r="B76">
-        <v>4207.7820000000002</v>
+        <v>4515.4269999999997</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -2159,7 +2168,7 @@
         <v>78</v>
       </c>
       <c r="B77">
-        <v>4304.7309999999998</v>
+        <v>4619.4579999999996</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -2170,7 +2179,7 @@
         <v>79</v>
       </c>
       <c r="B78">
-        <v>4409.518</v>
+        <v>4731.8879999999999</v>
       </c>
       <c r="C78">
         <v>0</v>
@@ -2181,7 +2190,7 @@
         <v>80</v>
       </c>
       <c r="B79">
-        <v>4424.5810000000001</v>
+        <v>4748.0460000000003</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -2192,7 +2201,7 @@
         <v>81</v>
       </c>
       <c r="B80">
-        <v>4462.0529999999999</v>
+        <v>4788.2539999999999</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -2203,7 +2212,7 @@
         <v>82</v>
       </c>
       <c r="B81">
-        <v>4498.66</v>
+        <v>4827.5370000000003</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -2214,7 +2223,7 @@
         <v>83</v>
       </c>
       <c r="B82">
-        <v>4538.4979999999996</v>
+        <v>4870.299</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -2225,7 +2234,7 @@
         <v>84</v>
       </c>
       <c r="B83">
-        <v>4541.28</v>
+        <v>4873.2870000000003</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -2236,7 +2245,7 @@
         <v>85</v>
       </c>
       <c r="B84">
-        <v>4584.2460000000001</v>
+        <v>4919.3919999999998</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -2247,7 +2256,7 @@
         <v>86</v>
       </c>
       <c r="B85">
-        <v>4618.8119999999999</v>
+        <v>4956.4769999999999</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -2258,7 +2267,7 @@
         <v>87</v>
       </c>
       <c r="B86">
-        <v>4713.0129999999999</v>
+        <v>5057.5529999999999</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -2269,7 +2278,7 @@
         <v>88</v>
       </c>
       <c r="B87">
-        <v>4791.7579999999998</v>
+        <v>5142.0330000000004</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -2280,7 +2289,7 @@
         <v>89</v>
       </c>
       <c r="B88">
-        <v>4828.8919999999998</v>
+        <v>5181.8590000000004</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -2291,7 +2300,7 @@
         <v>90</v>
       </c>
       <c r="B89">
-        <v>4847.8850000000002</v>
+        <v>5202.2120000000004</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -2302,7 +2311,7 @@
         <v>91</v>
       </c>
       <c r="B90">
-        <v>4923.76</v>
+        <v>5283.5969999999998</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -2313,7 +2322,7 @@
         <v>92</v>
       </c>
       <c r="B91">
-        <v>4938.7280000000001</v>
+        <v>5299.625</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -2324,7 +2333,7 @@
         <v>93</v>
       </c>
       <c r="B92">
-        <v>4971.3490000000002</v>
+        <v>5334.6</v>
       </c>
       <c r="C92">
         <v>0</v>
@@ -2335,7 +2344,7 @@
         <v>94</v>
       </c>
       <c r="B93">
-        <v>4947.1040000000003</v>
+        <v>5308.5559999999996</v>
       </c>
       <c r="C93">
         <v>0</v>
@@ -2346,7 +2355,7 @@
         <v>95</v>
       </c>
       <c r="B94">
-        <v>4939.759</v>
+        <v>5300.652</v>
       </c>
       <c r="C94">
         <v>1</v>
@@ -2357,7 +2366,7 @@
         <v>96</v>
       </c>
       <c r="B95">
-        <v>4946.7700000000004</v>
+        <v>5308.1639999999998</v>
       </c>
       <c r="C95">
         <v>1</v>
@@ -2368,7 +2377,7 @@
         <v>97</v>
       </c>
       <c r="B96">
-        <v>4992.357</v>
+        <v>5357.0770000000002</v>
       </c>
       <c r="C96">
         <v>1</v>
@@ -2379,7 +2388,7 @@
         <v>98</v>
       </c>
       <c r="B97">
-        <v>4938.857</v>
+        <v>5299.6719999999996</v>
       </c>
       <c r="C97">
         <v>1</v>
@@ -2390,7 +2399,7 @@
         <v>99</v>
       </c>
       <c r="B98">
-        <v>5072.9960000000001</v>
+        <v>5443.6189999999997</v>
       </c>
       <c r="C98">
         <v>0</v>
@@ -2401,7 +2410,7 @@
         <v>100</v>
       </c>
       <c r="B99">
-        <v>5100.4470000000001</v>
+        <v>5473.0590000000002</v>
       </c>
       <c r="C99">
         <v>0</v>
@@ -2412,7 +2421,7 @@
         <v>101</v>
       </c>
       <c r="B100">
-        <v>5142.4219999999996</v>
+        <v>5518.0720000000001</v>
       </c>
       <c r="C100">
         <v>0</v>
@@ -2423,7 +2432,7 @@
         <v>102</v>
       </c>
       <c r="B101">
-        <v>5154.5469999999996</v>
+        <v>5531.0320000000002</v>
       </c>
       <c r="C101">
         <v>0</v>
@@ -2434,7 +2443,7 @@
         <v>103</v>
       </c>
       <c r="B102">
-        <v>5249.3370000000004</v>
+        <v>5632.6490000000003</v>
       </c>
       <c r="C102">
         <v>0</v>
@@ -2445,7 +2454,7 @@
         <v>104</v>
       </c>
       <c r="B103">
-        <v>5368.4849999999997</v>
+        <v>5760.47</v>
       </c>
       <c r="C103">
         <v>0</v>
@@ -2456,7 +2465,7 @@
         <v>105</v>
       </c>
       <c r="B104">
-        <v>5419.1840000000002</v>
+        <v>5814.8540000000003</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -2467,7 +2476,7 @@
         <v>106</v>
       </c>
       <c r="B105">
-        <v>5509.9260000000004</v>
+        <v>5912.22</v>
       </c>
       <c r="C105">
         <v>0</v>
@@ -2478,7 +2487,7 @@
         <v>107</v>
       </c>
       <c r="B106">
-        <v>5646.2860000000001</v>
+        <v>6058.5439999999999</v>
       </c>
       <c r="C106">
         <v>0</v>
@@ -2489,7 +2498,7 @@
         <v>108</v>
       </c>
       <c r="B107">
-        <v>5707.7550000000001</v>
+        <v>6124.5060000000003</v>
       </c>
       <c r="C107">
         <v>0</v>
@@ -2500,7 +2509,7 @@
         <v>109</v>
       </c>
       <c r="B108">
-        <v>5677.7380000000003</v>
+        <v>6092.3010000000004</v>
       </c>
       <c r="C108">
         <v>0</v>
@@ -2511,7 +2520,7 @@
         <v>110</v>
       </c>
       <c r="B109">
-        <v>5731.6319999999996</v>
+        <v>6150.1310000000003</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -2522,7 +2531,7 @@
         <v>111</v>
       </c>
       <c r="B110">
-        <v>5682.3530000000001</v>
+        <v>6097.2579999999998</v>
       </c>
       <c r="C110">
         <v>1</v>
@@ -2533,7 +2542,7 @@
         <v>112</v>
       </c>
       <c r="B111">
-        <v>5695.8590000000004</v>
+        <v>6111.7510000000002</v>
       </c>
       <c r="C111">
         <v>1</v>
@@ -2544,7 +2553,7 @@
         <v>113</v>
       </c>
       <c r="B112">
-        <v>5642.0249999999996</v>
+        <v>6053.9780000000001</v>
       </c>
       <c r="C112">
         <v>1</v>
@@ -2555,7 +2564,7 @@
         <v>114</v>
       </c>
       <c r="B113">
-        <v>5620.1260000000002</v>
+        <v>6030.4639999999999</v>
       </c>
       <c r="C113">
         <v>1</v>
@@ -2566,7 +2575,7 @@
         <v>115</v>
       </c>
       <c r="B114">
-        <v>5551.7129999999997</v>
+        <v>5957.0349999999999</v>
       </c>
       <c r="C114">
         <v>1</v>
@@ -2577,7 +2586,7 @@
         <v>116</v>
       </c>
       <c r="B115">
-        <v>5591.3819999999996</v>
+        <v>5999.61</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -2588,7 +2597,7 @@
         <v>117</v>
       </c>
       <c r="B116">
-        <v>5687.0870000000004</v>
+        <v>6102.326</v>
       </c>
       <c r="C116">
         <v>0</v>
@@ -2599,7 +2608,7 @@
         <v>118</v>
       </c>
       <c r="B117">
-        <v>5763.665</v>
+        <v>6184.53</v>
       </c>
       <c r="C117">
         <v>0</v>
@@ -2610,7 +2619,7 @@
         <v>119</v>
       </c>
       <c r="B118">
-        <v>5893.2759999999998</v>
+        <v>6323.6490000000003</v>
       </c>
       <c r="C118">
         <v>0</v>
@@ -2621,7 +2630,7 @@
         <v>120</v>
       </c>
       <c r="B119">
-        <v>5936.5150000000003</v>
+        <v>6370.0249999999996</v>
       </c>
       <c r="C119">
         <v>0</v>
@@ -2632,7 +2641,7 @@
         <v>121</v>
       </c>
       <c r="B120">
-        <v>5969.0889999999999</v>
+        <v>6404.8950000000004</v>
       </c>
       <c r="C120">
         <v>0</v>
@@ -2643,7 +2652,7 @@
         <v>122</v>
       </c>
       <c r="B121">
-        <v>6012.3559999999998</v>
+        <v>6451.1769999999997</v>
       </c>
       <c r="C121">
         <v>0</v>
@@ -2654,7 +2663,7 @@
         <v>123</v>
       </c>
       <c r="B122">
-        <v>6083.3909999999996</v>
+        <v>6527.7030000000004</v>
       </c>
       <c r="C122">
         <v>0</v>
@@ -2665,7 +2674,7 @@
         <v>124</v>
       </c>
       <c r="B123">
-        <v>6201.6589999999997</v>
+        <v>6654.4660000000003</v>
       </c>
       <c r="C123">
         <v>0</v>
@@ -2676,7 +2685,7 @@
         <v>125</v>
       </c>
       <c r="B124">
-        <v>6313.5590000000002</v>
+        <v>6774.4570000000003</v>
       </c>
       <c r="C124">
         <v>0</v>
@@ -2687,7 +2696,7 @@
         <v>126</v>
       </c>
       <c r="B125">
-        <v>6313.6970000000001</v>
+        <v>6774.5919999999996</v>
       </c>
       <c r="C125">
         <v>0</v>
@@ -2698,7 +2707,7 @@
         <v>127</v>
       </c>
       <c r="B126">
-        <v>6333.848</v>
+        <v>6796.26</v>
       </c>
       <c r="C126">
         <v>0</v>
@@ -2709,7 +2718,7 @@
         <v>128</v>
       </c>
       <c r="B127">
-        <v>6578.6049999999996</v>
+        <v>7058.92</v>
       </c>
       <c r="C127">
         <v>0</v>
@@ -2720,7 +2729,7 @@
         <v>129</v>
       </c>
       <c r="B128">
-        <v>6644.7539999999999</v>
+        <v>7129.915</v>
       </c>
       <c r="C128">
         <v>0</v>
@@ -2731,7 +2740,7 @@
         <v>130</v>
       </c>
       <c r="B129">
-        <v>6734.0690000000004</v>
+        <v>7225.75</v>
       </c>
       <c r="C129">
         <v>0</v>
@@ -2742,7 +2751,7 @@
         <v>131</v>
       </c>
       <c r="B130">
-        <v>6746.1760000000004</v>
+        <v>7238.7269999999999</v>
       </c>
       <c r="C130">
         <v>0</v>
@@ -2753,7 +2762,7 @@
         <v>132</v>
       </c>
       <c r="B131">
-        <v>6753.3890000000001</v>
+        <v>7246.4539999999997</v>
       </c>
       <c r="C131">
         <v>0</v>
@@ -2764,7 +2773,7 @@
         <v>133</v>
       </c>
       <c r="B132">
-        <v>6803.558</v>
+        <v>7300.2809999999999</v>
       </c>
       <c r="C132">
         <v>0</v>
@@ -2775,7 +2784,7 @@
         <v>134</v>
       </c>
       <c r="B133">
-        <v>6820.5720000000001</v>
+        <v>7318.5349999999999</v>
       </c>
       <c r="C133">
         <v>0</v>
@@ -2786,7 +2795,7 @@
         <v>135</v>
       </c>
       <c r="B134">
-        <v>6842.0240000000003</v>
+        <v>7341.5569999999998</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -2797,7 +2806,7 @@
         <v>136</v>
       </c>
       <c r="B135">
-        <v>6701.0460000000003</v>
+        <v>7190.2889999999998</v>
       </c>
       <c r="C135">
         <v>1</v>
@@ -2808,7 +2817,7 @@
         <v>137</v>
       </c>
       <c r="B136">
-        <v>6693.0820000000003</v>
+        <v>7181.7430000000004</v>
       </c>
       <c r="C136">
         <v>1</v>
@@ -2819,7 +2828,7 @@
         <v>138</v>
       </c>
       <c r="B137">
-        <v>6817.9030000000002</v>
+        <v>7315.6769999999997</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -2830,7 +2839,7 @@
         <v>139</v>
       </c>
       <c r="B138">
-        <v>6951.4949999999999</v>
+        <v>7459.0219999999999</v>
       </c>
       <c r="C138">
         <v>0</v>
@@ -2841,7 +2850,7 @@
         <v>140</v>
       </c>
       <c r="B139">
-        <v>6899.98</v>
+        <v>7403.7449999999999</v>
       </c>
       <c r="C139">
         <v>0</v>
@@ -2852,7 +2861,7 @@
         <v>141</v>
       </c>
       <c r="B140">
-        <v>6982.6090000000004</v>
+        <v>7492.4049999999997</v>
       </c>
       <c r="C140">
         <v>0</v>
@@ -2863,7 +2872,7 @@
         <v>142</v>
       </c>
       <c r="B141">
-        <v>6906.5290000000005</v>
+        <v>7410.768</v>
       </c>
       <c r="C141">
         <v>1</v>
@@ -2874,7 +2883,7 @@
         <v>143</v>
       </c>
       <c r="B142">
-        <v>6799.2330000000002</v>
+        <v>7295.6310000000003</v>
       </c>
       <c r="C142">
         <v>1</v>
@@ -2885,7 +2894,7 @@
         <v>144</v>
       </c>
       <c r="B143">
-        <v>6830.2510000000002</v>
+        <v>7328.9120000000003</v>
       </c>
       <c r="C143">
         <v>1</v>
@@ -2896,7 +2905,7 @@
         <v>145</v>
       </c>
       <c r="B144">
-        <v>6804.1390000000001</v>
+        <v>7300.8959999999997</v>
       </c>
       <c r="C144">
         <v>1</v>
@@ -2907,7 +2916,7 @@
         <v>146</v>
       </c>
       <c r="B145">
-        <v>6806.857</v>
+        <v>7303.817</v>
       </c>
       <c r="C145">
         <v>1</v>
@@ -2918,7 +2927,7 @@
         <v>147</v>
       </c>
       <c r="B146">
-        <v>6896.5609999999997</v>
+        <v>7400.0659999999998</v>
       </c>
       <c r="C146">
         <v>0</v>
@@ -2929,7 +2938,7 @@
         <v>148</v>
       </c>
       <c r="B147">
-        <v>7053.5</v>
+        <v>7568.4560000000001</v>
       </c>
       <c r="C147">
         <v>0</v>
@@ -2940,7 +2949,7 @@
         <v>149</v>
       </c>
       <c r="B148">
-        <v>7194.5039999999999</v>
+        <v>7719.7460000000001</v>
       </c>
       <c r="C148">
         <v>0</v>
@@ -2951,7 +2960,7 @@
         <v>150</v>
       </c>
       <c r="B149">
-        <v>7344.5969999999998</v>
+        <v>7880.7939999999999</v>
       </c>
       <c r="C149">
         <v>0</v>
@@ -2962,7 +2971,7 @@
         <v>151</v>
       </c>
       <c r="B150">
-        <v>7488.1670000000004</v>
+        <v>8034.8469999999998</v>
       </c>
       <c r="C150">
         <v>0</v>
@@ -2973,7 +2982,7 @@
         <v>152</v>
       </c>
       <c r="B151">
-        <v>7617.5469999999996</v>
+        <v>8173.67</v>
       </c>
       <c r="C151">
         <v>0</v>
@@ -2984,7 +2993,7 @@
         <v>153</v>
       </c>
       <c r="B152">
-        <v>7690.9849999999997</v>
+        <v>8252.4650000000001</v>
       </c>
       <c r="C152">
         <v>0</v>
@@ -2995,7 +3004,7 @@
         <v>154</v>
       </c>
       <c r="B153">
-        <v>7754.1170000000002</v>
+        <v>8320.1990000000005</v>
       </c>
       <c r="C153">
         <v>0</v>
@@ -3006,7 +3015,7 @@
         <v>155</v>
       </c>
       <c r="B154">
-        <v>7829.26</v>
+        <v>8400.82</v>
       </c>
       <c r="C154">
         <v>0</v>
@@ -3017,7 +3026,7 @@
         <v>156</v>
       </c>
       <c r="B155">
-        <v>7898.1940000000004</v>
+        <v>8474.7870000000003</v>
       </c>
       <c r="C155">
         <v>0</v>
@@ -3028,7 +3037,7 @@
         <v>157</v>
       </c>
       <c r="B156">
-        <v>8018.8090000000002</v>
+        <v>8604.2199999999993</v>
       </c>
       <c r="C156">
         <v>0</v>
@@ -3039,7 +3048,7 @@
         <v>158</v>
       </c>
       <c r="B157">
-        <v>8078.415</v>
+        <v>8668.1880000000001</v>
       </c>
       <c r="C157">
         <v>0</v>
@@ -3050,7 +3059,7 @@
         <v>159</v>
       </c>
       <c r="B158">
-        <v>8153.8289999999997</v>
+        <v>8749.1270000000004</v>
       </c>
       <c r="C158">
         <v>0</v>
@@ -3061,7 +3070,7 @@
         <v>160</v>
       </c>
       <c r="B159">
-        <v>8190.5519999999997</v>
+        <v>8788.5239999999994</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -3072,7 +3081,7 @@
         <v>161</v>
       </c>
       <c r="B160">
-        <v>8268.9349999999995</v>
+        <v>8872.6010000000006</v>
       </c>
       <c r="C160">
         <v>0</v>
@@ -3083,7 +3092,7 @@
         <v>162</v>
       </c>
       <c r="B161">
-        <v>8313.3379999999997</v>
+        <v>8920.1929999999993</v>
       </c>
       <c r="C161">
         <v>0</v>
@@ -3094,7 +3103,7 @@
         <v>163</v>
       </c>
       <c r="B162">
-        <v>8375.2739999999994</v>
+        <v>8986.3670000000002</v>
       </c>
       <c r="C162">
         <v>0</v>
@@ -3105,7 +3114,7 @@
         <v>164</v>
       </c>
       <c r="B163">
-        <v>8465.6299999999992</v>
+        <v>9083.2559999999994</v>
       </c>
       <c r="C163">
         <v>0</v>
@@ -3116,7 +3125,7 @@
         <v>165</v>
       </c>
       <c r="B164">
-        <v>8539.0750000000007</v>
+        <v>9162.0239999999994</v>
       </c>
       <c r="C164">
         <v>0</v>
@@ -3127,7 +3136,7 @@
         <v>166</v>
       </c>
       <c r="B165">
-        <v>8685.6939999999995</v>
+        <v>9319.3320000000003</v>
       </c>
       <c r="C165">
         <v>0</v>
@@ -3138,7 +3147,7 @@
         <v>167</v>
       </c>
       <c r="B166">
-        <v>8730.5689999999995</v>
+        <v>9367.5020000000004</v>
       </c>
       <c r="C166">
         <v>0</v>
@@ -3149,7 +3158,7 @@
         <v>168</v>
       </c>
       <c r="B167">
-        <v>8845.2800000000007</v>
+        <v>9490.5939999999991</v>
       </c>
       <c r="C167">
         <v>0</v>
@@ -3160,7 +3169,7 @@
         <v>169</v>
       </c>
       <c r="B168">
-        <v>8897.107</v>
+        <v>9546.2060000000001</v>
       </c>
       <c r="C168">
         <v>0</v>
@@ -3171,7 +3180,7 @@
         <v>170</v>
       </c>
       <c r="B169">
-        <v>9015.6610000000001</v>
+        <v>9673.4050000000007</v>
       </c>
       <c r="C169">
         <v>0</v>
@@ -3182,7 +3191,7 @@
         <v>171</v>
       </c>
       <c r="B170">
-        <v>9107.3140000000003</v>
+        <v>9771.7250000000004</v>
       </c>
       <c r="C170">
         <v>0</v>
@@ -3193,7 +3202,7 @@
         <v>172</v>
       </c>
       <c r="B171">
-        <v>9176.8269999999993</v>
+        <v>9846.2929999999997</v>
       </c>
       <c r="C171">
         <v>0</v>
@@ -3204,7 +3213,7 @@
         <v>173</v>
       </c>
       <c r="B172">
-        <v>9244.8160000000007</v>
+        <v>9919.2279999999992</v>
       </c>
       <c r="C172">
         <v>0</v>
@@ -3215,7 +3224,7 @@
         <v>174</v>
       </c>
       <c r="B173">
-        <v>9263.0329999999994</v>
+        <v>9938.7669999999998</v>
       </c>
       <c r="C173">
         <v>0</v>
@@ -3226,7 +3235,7 @@
         <v>175</v>
       </c>
       <c r="B174">
-        <v>9364.259</v>
+        <v>10047.386</v>
       </c>
       <c r="C174">
         <v>0</v>
@@ -3237,7 +3246,7 @@
         <v>176</v>
       </c>
       <c r="B175">
-        <v>9398.2430000000004</v>
+        <v>10083.855</v>
       </c>
       <c r="C175">
         <v>0</v>
@@ -3248,7 +3257,7 @@
         <v>177</v>
       </c>
       <c r="B176">
-        <v>9404.4940000000006</v>
+        <v>10090.569</v>
       </c>
       <c r="C176">
         <v>0</v>
@@ -3259,7 +3268,7 @@
         <v>178</v>
       </c>
       <c r="B177">
-        <v>9318.8760000000002</v>
+        <v>9998.7039999999997</v>
       </c>
       <c r="C177">
         <v>1</v>
@@ -3270,7 +3279,7 @@
         <v>179</v>
       </c>
       <c r="B178">
-        <v>9275.2759999999998</v>
+        <v>9951.9159999999993</v>
       </c>
       <c r="C178">
         <v>1</v>
@@ -3281,7 +3290,7 @@
         <v>180</v>
       </c>
       <c r="B179">
-        <v>9347.5969999999998</v>
+        <v>10029.51</v>
       </c>
       <c r="C179">
         <v>0</v>
@@ -3292,7 +3301,7 @@
         <v>181</v>
       </c>
       <c r="B180">
-        <v>9394.8340000000007</v>
+        <v>10080.195</v>
       </c>
       <c r="C180">
         <v>0</v>
@@ -3303,7 +3312,7 @@
         <v>182</v>
       </c>
       <c r="B181">
-        <v>9427.5810000000001</v>
+        <v>10115.329</v>
       </c>
       <c r="C181">
         <v>0</v>
@@ -3314,7 +3323,7 @@
         <v>183</v>
       </c>
       <c r="B182">
-        <v>9540.4439999999995</v>
+        <v>10236.434999999999</v>
       </c>
       <c r="C182">
         <v>0</v>
@@ -3325,7 +3334,7 @@
         <v>184</v>
       </c>
       <c r="B183">
-        <v>9643.893</v>
+        <v>10347.429</v>
       </c>
       <c r="C183">
         <v>0</v>
@@ -3336,7 +3345,7 @@
         <v>185</v>
       </c>
       <c r="B184">
-        <v>9739.1849999999995</v>
+        <v>10449.673000000001</v>
       </c>
       <c r="C184">
         <v>0</v>
@@ -3347,7 +3356,7 @@
         <v>186</v>
       </c>
       <c r="B185">
-        <v>9840.7530000000006</v>
+        <v>10558.647999999999</v>
       </c>
       <c r="C185">
         <v>0</v>
@@ -3358,7 +3367,7 @@
         <v>187</v>
       </c>
       <c r="B186">
-        <v>9857.1849999999995</v>
+        <v>10576.275</v>
       </c>
       <c r="C186">
         <v>0</v>
@@ -3369,7 +3378,7 @@
         <v>188</v>
       </c>
       <c r="B187">
-        <v>9914.5650000000005</v>
+        <v>10637.847</v>
       </c>
       <c r="C187">
         <v>0</v>
@@ -3380,7 +3389,7 @@
         <v>189</v>
       </c>
       <c r="B188">
-        <v>9961.8729999999996</v>
+        <v>10688.606</v>
       </c>
       <c r="C188">
         <v>0</v>
@@ -3391,7 +3400,7 @@
         <v>190</v>
       </c>
       <c r="B189">
-        <v>10097.361999999999</v>
+        <v>10833.986999999999</v>
       </c>
       <c r="C189">
         <v>0</v>
@@ -3402,7 +3411,7 @@
         <v>191</v>
       </c>
       <c r="B190">
-        <v>10195.338</v>
+        <v>10939.116</v>
       </c>
       <c r="C190">
         <v>0</v>
@@ -3413,7 +3422,7 @@
         <v>192</v>
       </c>
       <c r="B191">
-        <v>10333.495000000001</v>
+        <v>11087.361000000001</v>
       </c>
       <c r="C191">
         <v>0</v>
@@ -3424,7 +3433,7 @@
         <v>193</v>
       </c>
       <c r="B192">
-        <v>10393.897999999999</v>
+        <v>11152.175999999999</v>
       </c>
       <c r="C192">
         <v>0</v>
@@ -3435,7 +3444,7 @@
         <v>194</v>
       </c>
       <c r="B193">
-        <v>10512.962</v>
+        <v>11279.932000000001</v>
       </c>
       <c r="C193">
         <v>0</v>
@@ -3446,7 +3455,7 @@
         <v>195</v>
       </c>
       <c r="B194">
-        <v>10550.251</v>
+        <v>11319.950999999999</v>
       </c>
       <c r="C194">
         <v>0</v>
@@ -3457,7 +3466,7 @@
         <v>196</v>
       </c>
       <c r="B195">
-        <v>10581.723</v>
+        <v>11353.721</v>
       </c>
       <c r="C195">
         <v>0</v>
@@ -3468,7 +3477,7 @@
         <v>197</v>
       </c>
       <c r="B196">
-        <v>10671.737999999999</v>
+        <v>11450.31</v>
       </c>
       <c r="C196">
         <v>0</v>
@@ -3479,7 +3488,7 @@
         <v>198</v>
       </c>
       <c r="B197">
-        <v>10744.203</v>
+        <v>11528.066999999999</v>
       </c>
       <c r="C197">
         <v>0</v>
@@ -3490,7 +3499,7 @@
         <v>199</v>
       </c>
       <c r="B198">
-        <v>10824.674000000001</v>
+        <v>11614.418</v>
       </c>
       <c r="C198">
         <v>0</v>
@@ -3501,7 +3510,7 @@
         <v>200</v>
       </c>
       <c r="B199">
-        <v>11005.217000000001</v>
+        <v>11808.14</v>
       </c>
       <c r="C199">
         <v>0</v>
@@ -3512,7 +3521,7 @@
         <v>201</v>
       </c>
       <c r="B200">
-        <v>11103.934999999999</v>
+        <v>11914.063</v>
       </c>
       <c r="C200">
         <v>0</v>
@@ -3523,7 +3532,7 @@
         <v>202</v>
       </c>
       <c r="B201">
-        <v>11219.237999999999</v>
+        <v>12037.775</v>
       </c>
       <c r="C201">
         <v>0</v>
@@ -3534,7 +3543,7 @@
         <v>203</v>
       </c>
       <c r="B202">
-        <v>11291.665000000001</v>
+        <v>12115.472</v>
       </c>
       <c r="C202">
         <v>0</v>
@@ -3545,7 +3554,7 @@
         <v>204</v>
       </c>
       <c r="B203">
-        <v>11479.33</v>
+        <v>12317.221</v>
       </c>
       <c r="C203">
         <v>0</v>
@@ -3556,7 +3565,7 @@
         <v>205</v>
       </c>
       <c r="B204">
-        <v>11622.911</v>
+        <v>12471.01</v>
       </c>
       <c r="C204">
         <v>0</v>
@@ -3567,7 +3576,7 @@
         <v>206</v>
       </c>
       <c r="B205">
-        <v>11722.722</v>
+        <v>12577.495000000001</v>
       </c>
       <c r="C205">
         <v>0</v>
@@ -3578,7 +3587,7 @@
         <v>207</v>
       </c>
       <c r="B206">
-        <v>11839.876</v>
+        <v>12703.742</v>
       </c>
       <c r="C206">
         <v>0</v>
@@ -3589,7 +3598,7 @@
         <v>208</v>
       </c>
       <c r="B207">
-        <v>11949.492</v>
+        <v>12821.339</v>
       </c>
       <c r="C207">
         <v>0</v>
@@ -3600,7 +3609,7 @@
         <v>209</v>
       </c>
       <c r="B208">
-        <v>12099.191000000001</v>
+        <v>12982.752</v>
       </c>
       <c r="C208">
         <v>0</v>
@@ -3611,7 +3620,7 @@
         <v>210</v>
       </c>
       <c r="B209">
-        <v>12294.736999999999</v>
+        <v>13191.67</v>
       </c>
       <c r="C209">
         <v>0</v>
@@ -3622,7 +3631,7 @@
         <v>211</v>
       </c>
       <c r="B210">
-        <v>12410.778</v>
+        <v>13315.597</v>
       </c>
       <c r="C210">
         <v>0</v>
@@ -3633,7 +3642,7 @@
         <v>212</v>
       </c>
       <c r="B211">
-        <v>12514.407999999999</v>
+        <v>13426.748</v>
       </c>
       <c r="C211">
         <v>0</v>
@@ -3644,7 +3653,7 @@
         <v>213</v>
       </c>
       <c r="B212">
-        <v>12679.977000000001</v>
+        <v>13604.771000000001</v>
       </c>
       <c r="C212">
         <v>0</v>
@@ -3655,7 +3664,7 @@
         <v>214</v>
       </c>
       <c r="B213">
-        <v>12888.281000000001</v>
+        <v>13827.98</v>
       </c>
       <c r="C213">
         <v>0</v>
@@ -3666,7 +3675,7 @@
         <v>215</v>
       </c>
       <c r="B214">
-        <v>12935.252</v>
+        <v>13878.147000000001</v>
       </c>
       <c r="C214">
         <v>0</v>
@@ -3677,7 +3686,7 @@
         <v>216</v>
       </c>
       <c r="B215">
-        <v>13170.749</v>
+        <v>14130.907999999999</v>
       </c>
       <c r="C215">
         <v>0</v>
@@ -3688,7 +3697,7 @@
         <v>217</v>
       </c>
       <c r="B216">
-        <v>13183.89</v>
+        <v>14145.312</v>
       </c>
       <c r="C216">
         <v>0</v>
@@ -3699,7 +3708,7 @@
         <v>218</v>
       </c>
       <c r="B217">
-        <v>13262.25</v>
+        <v>14229.764999999999</v>
       </c>
       <c r="C217">
         <v>0</v>
@@ -3710,7 +3719,7 @@
         <v>219</v>
       </c>
       <c r="B218">
-        <v>13219.251</v>
+        <v>14183.12</v>
       </c>
       <c r="C218">
         <v>0</v>
@@ -3721,7 +3730,7 @@
         <v>220</v>
       </c>
       <c r="B219">
-        <v>13301.394</v>
+        <v>14271.694</v>
       </c>
       <c r="C219">
         <v>1</v>
@@ -3732,7 +3741,7 @@
         <v>221</v>
       </c>
       <c r="B220">
-        <v>13248.142</v>
+        <v>14214.516</v>
       </c>
       <c r="C220">
         <v>1</v>
@@ -3743,7 +3752,7 @@
         <v>222</v>
       </c>
       <c r="B221">
-        <v>13284.880999999999</v>
+        <v>14253.574000000001</v>
       </c>
       <c r="C221">
         <v>1</v>
@@ -3754,7 +3763,7 @@
         <v>223</v>
       </c>
       <c r="B222">
-        <v>13394.91</v>
+        <v>14372.785</v>
       </c>
       <c r="C222">
         <v>0</v>
@@ -3765,7 +3774,7 @@
         <v>224</v>
       </c>
       <c r="B223">
-        <v>13477.356</v>
+        <v>14460.848</v>
       </c>
       <c r="C223">
         <v>0</v>
@@ -3776,7 +3785,7 @@
         <v>225</v>
       </c>
       <c r="B224">
-        <v>13531.741</v>
+        <v>14519.633</v>
       </c>
       <c r="C224">
         <v>0</v>
@@ -3787,7 +3796,7 @@
         <v>226</v>
       </c>
       <c r="B225">
-        <v>13549.421</v>
+        <v>14537.58</v>
       </c>
       <c r="C225">
         <v>0</v>
@@ -3798,7 +3807,7 @@
         <v>227</v>
       </c>
       <c r="B226">
-        <v>13619.433999999999</v>
+        <v>14614.141</v>
       </c>
       <c r="C226">
         <v>0</v>
@@ -3809,7 +3818,7 @@
         <v>228</v>
       </c>
       <c r="B227">
-        <v>13741.107</v>
+        <v>14743.566999999999</v>
       </c>
       <c r="C227">
         <v>0</v>
@@ -3820,7 +3829,7 @@
         <v>229</v>
       </c>
       <c r="B228">
-        <v>13970.156999999999</v>
+        <v>14988.781999999999</v>
       </c>
       <c r="C228">
         <v>0</v>
@@ -3831,7 +3840,7 @@
         <v>230</v>
       </c>
       <c r="B229">
-        <v>14131.379000000001</v>
+        <v>15162.76</v>
       </c>
       <c r="C229">
         <v>0</v>
@@ -3842,7 +3851,7 @@
         <v>231</v>
       </c>
       <c r="B230">
-        <v>14212.34</v>
+        <v>15248.68</v>
       </c>
       <c r="C230">
         <v>0</v>
@@ -3853,7 +3862,7 @@
         <v>232</v>
       </c>
       <c r="B231">
-        <v>14323.017</v>
+        <v>15366.85</v>
       </c>
       <c r="C231">
         <v>0</v>
@@ -3864,7 +3873,7 @@
         <v>233</v>
       </c>
       <c r="B232">
-        <v>14457.832</v>
+        <v>15512.619000000001</v>
       </c>
       <c r="C232">
         <v>0</v>
@@ -3875,7 +3884,7 @@
         <v>234</v>
       </c>
       <c r="B233">
-        <v>14605.594999999999</v>
+        <v>15670.88</v>
       </c>
       <c r="C233">
         <v>0</v>
@@ -3886,7 +3895,7 @@
         <v>235</v>
       </c>
       <c r="B234">
-        <v>14767.846</v>
+        <v>15844.727000000001</v>
       </c>
       <c r="C234">
         <v>0</v>
@@ -3897,7 +3906,7 @@
         <v>236</v>
       </c>
       <c r="B235">
-        <v>14839.707</v>
+        <v>15922.781999999999</v>
       </c>
       <c r="C235">
         <v>0</v>
@@ -3908,7 +3917,7 @@
         <v>237</v>
       </c>
       <c r="B236">
-        <v>14956.290999999999</v>
+        <v>16047.587</v>
       </c>
       <c r="C236">
         <v>0</v>
@@ -3919,7 +3928,7 @@
         <v>238</v>
       </c>
       <c r="B237">
-        <v>15041.232</v>
+        <v>16136.734</v>
       </c>
       <c r="C237">
         <v>0</v>
@@ -3930,7 +3939,7 @@
         <v>239</v>
       </c>
       <c r="B238">
-        <v>15244.088</v>
+        <v>16353.834999999999</v>
       </c>
       <c r="C238">
         <v>0</v>
@@ -3941,7 +3950,7 @@
         <v>240</v>
       </c>
       <c r="B239">
-        <v>15281.525</v>
+        <v>16396.151000000002</v>
       </c>
       <c r="C239">
         <v>0</v>
@@ -3952,7 +3961,7 @@
         <v>241</v>
       </c>
       <c r="B240">
-        <v>15304.517</v>
+        <v>16420.738000000001</v>
       </c>
       <c r="C240">
         <v>0</v>
@@ -3963,7 +3972,7 @@
         <v>242</v>
       </c>
       <c r="B241">
-        <v>15433.643</v>
+        <v>16561.866000000002</v>
       </c>
       <c r="C241">
         <v>0</v>
@@ -3974,7 +3983,7 @@
         <v>243</v>
       </c>
       <c r="B242">
-        <v>15478.956</v>
+        <v>16611.689999999999</v>
       </c>
       <c r="C242">
         <v>0</v>
@@ -3985,7 +3994,7 @@
         <v>244</v>
       </c>
       <c r="B243">
-        <v>15577.779</v>
+        <v>16713.313999999998</v>
       </c>
       <c r="C243">
         <v>0</v>
@@ -3996,7 +4005,7 @@
         <v>245</v>
       </c>
       <c r="B244">
-        <v>15671.605</v>
+        <v>16809.587</v>
       </c>
       <c r="C244">
         <v>0</v>
@@ -4007,7 +4016,7 @@
         <v>246</v>
       </c>
       <c r="B245">
-        <v>15767.146000000001</v>
+        <v>16915.190999999999</v>
       </c>
       <c r="C245">
         <v>0</v>
@@ -4018,7 +4027,7 @@
         <v>247</v>
       </c>
       <c r="B246">
-        <v>15702.906000000001</v>
+        <v>16843.003000000001</v>
       </c>
       <c r="C246">
         <v>1</v>
@@ -4029,7 +4038,7 @@
         <v>248</v>
       </c>
       <c r="B247">
-        <v>15792.772999999999</v>
+        <v>16943.291000000001</v>
       </c>
       <c r="C247">
         <v>1</v>
@@ -4040,7 +4049,7 @@
         <v>249</v>
       </c>
       <c r="B248">
-        <v>15709.562</v>
+        <v>16854.294999999998</v>
       </c>
       <c r="C248">
         <v>1</v>
@@ -4051,7 +4060,7 @@
         <v>250</v>
       </c>
       <c r="B249">
-        <v>15366.607</v>
+        <v>16485.349999999999</v>
       </c>
       <c r="C249">
         <v>1</v>
@@ -4062,7 +4071,7 @@
         <v>251</v>
       </c>
       <c r="B250">
-        <v>15187.475</v>
+        <v>16298.262000000001</v>
       </c>
       <c r="C250">
         <v>1</v>
@@ -4073,7 +4082,7 @@
         <v>252</v>
       </c>
       <c r="B251">
-        <v>15161.772000000001</v>
+        <v>16269.145</v>
       </c>
       <c r="C251">
         <v>1</v>
@@ -4084,7 +4093,7 @@
         <v>253</v>
       </c>
       <c r="B252">
-        <v>15216.647000000001</v>
+        <v>16326.281000000001</v>
       </c>
       <c r="C252">
         <v>0</v>
@@ -4095,7 +4104,7 @@
         <v>254</v>
       </c>
       <c r="B253">
-        <v>15379.155000000001</v>
+        <v>16502.754000000001</v>
       </c>
       <c r="C253">
         <v>0</v>
@@ -4106,7 +4115,7 @@
         <v>255</v>
       </c>
       <c r="B254">
-        <v>15456.058999999999</v>
+        <v>16582.71</v>
       </c>
       <c r="C254">
         <v>0</v>
@@ -4117,7 +4126,7 @@
         <v>256</v>
       </c>
       <c r="B255">
-        <v>15605.628000000001</v>
+        <v>16743.162</v>
       </c>
       <c r="C255">
         <v>0</v>
@@ -4128,7 +4137,7 @@
         <v>257</v>
       </c>
       <c r="B256">
-        <v>15726.281999999999</v>
+        <v>16872.266</v>
       </c>
       <c r="C256">
         <v>0</v>
@@ -4139,7 +4148,7 @@
         <v>258</v>
       </c>
       <c r="B257">
-        <v>15807.995000000001</v>
+        <v>16960.864000000001</v>
       </c>
       <c r="C257">
         <v>0</v>
@@ -4150,7 +4159,7 @@
         <v>259</v>
       </c>
       <c r="B258">
-        <v>15769.911</v>
+        <v>16920.632000000001</v>
       </c>
       <c r="C258">
         <v>0</v>
@@ -4161,7 +4170,7 @@
         <v>260</v>
       </c>
       <c r="B259">
-        <v>15876.839</v>
+        <v>17035.114000000001</v>
       </c>
       <c r="C259">
         <v>0</v>
@@ -4172,7 +4181,7 @@
         <v>261</v>
       </c>
       <c r="B260">
-        <v>15870.683999999999</v>
+        <v>17031.312999999998</v>
       </c>
       <c r="C260">
         <v>0</v>
@@ -4183,7 +4192,7 @@
         <v>262</v>
       </c>
       <c r="B261">
-        <v>16048.701999999999</v>
+        <v>17222.582999999999</v>
       </c>
       <c r="C261">
         <v>0</v>
@@ -4194,7 +4203,7 @@
         <v>263</v>
       </c>
       <c r="B262">
-        <v>16179.968000000001</v>
+        <v>17367.009999999998</v>
       </c>
       <c r="C262">
         <v>0</v>
@@ -4205,7 +4214,7 @@
         <v>264</v>
       </c>
       <c r="B263">
-        <v>16253.726000000001</v>
+        <v>17444.525000000001</v>
       </c>
       <c r="C263">
         <v>0</v>
@@ -4216,7 +4225,7 @@
         <v>265</v>
       </c>
       <c r="B264">
-        <v>16282.151</v>
+        <v>17469.650000000001</v>
       </c>
       <c r="C264">
         <v>0</v>
@@ -4227,7 +4236,7 @@
         <v>266</v>
       </c>
       <c r="B265">
-        <v>16300.035</v>
+        <v>17489.851999999999</v>
       </c>
       <c r="C265">
         <v>0</v>
@@ -4238,7 +4247,7 @@
         <v>267</v>
       </c>
       <c r="B266">
-        <v>16441.485000000001</v>
+        <v>17662.400000000001</v>
       </c>
       <c r="C266">
         <v>0</v>
@@ -4249,7 +4258,7 @@
         <v>268</v>
       </c>
       <c r="B267">
-        <v>16464.401999999998</v>
+        <v>17709.670999999998</v>
       </c>
       <c r="C267">
         <v>0</v>
@@ -4260,7 +4269,7 @@
         <v>269</v>
       </c>
       <c r="B268">
-        <v>16594.742999999999</v>
+        <v>17860.45</v>
       </c>
       <c r="C268">
         <v>0</v>
@@ -4271,7 +4280,7 @@
         <v>270</v>
       </c>
       <c r="B269">
-        <v>16712.759999999998</v>
+        <v>18016.147000000001</v>
       </c>
       <c r="C269">
         <v>0</v>
@@ -4282,7 +4291,7 @@
         <v>271</v>
       </c>
       <c r="B270">
-        <v>16654.246999999999</v>
+        <v>17953.973999999998</v>
       </c>
       <c r="C270">
         <v>0</v>
@@ -4293,7 +4302,7 @@
         <v>272</v>
       </c>
       <c r="B271">
-        <v>16868.109</v>
+        <v>18185.911</v>
       </c>
       <c r="C271">
         <v>0</v>
@@ -4304,7 +4313,7 @@
         <v>273</v>
       </c>
       <c r="B272">
-        <v>17064.616000000002</v>
+        <v>18406.940999999999</v>
       </c>
       <c r="C272">
         <v>0</v>
@@ -4315,7 +4324,7 @@
         <v>274</v>
       </c>
       <c r="B273">
-        <v>17141.235000000001</v>
+        <v>18500.030999999999</v>
       </c>
       <c r="C273">
         <v>0</v>
@@ -4326,7 +4335,7 @@
         <v>275</v>
       </c>
       <c r="B274">
-        <v>17280.647000000001</v>
+        <v>18666.620999999999</v>
       </c>
       <c r="C274">
         <v>0</v>
@@ -4337,7 +4346,7 @@
         <v>276</v>
       </c>
       <c r="B275">
-        <v>17380.875</v>
+        <v>18782.242999999999</v>
       </c>
       <c r="C275">
         <v>0</v>
@@ -4348,7 +4357,7 @@
         <v>277</v>
       </c>
       <c r="B276">
-        <v>17437.080000000002</v>
+        <v>18857.418000000001</v>
       </c>
       <c r="C276">
         <v>0</v>
@@ -4359,7 +4368,7 @@
         <v>278</v>
       </c>
       <c r="B277">
-        <v>17462.579000000002</v>
+        <v>18892.205999999998</v>
       </c>
       <c r="C277">
         <v>0</v>
@@ -4370,7 +4379,7 @@
         <v>279</v>
       </c>
       <c r="B278">
-        <v>17565.465</v>
+        <v>19001.689999999999</v>
       </c>
       <c r="C278">
         <v>0</v>
@@ -4381,7 +4390,7 @@
         <v>280</v>
       </c>
       <c r="B279">
-        <v>17618.580999999998</v>
+        <v>19062.708999999999</v>
       </c>
       <c r="C279">
         <v>0</v>
@@ -4392,7 +4401,7 @@
         <v>281</v>
       </c>
       <c r="B280">
-        <v>17724.489000000001</v>
+        <v>19197.937999999998</v>
       </c>
       <c r="C280">
         <v>0</v>
@@ -4403,7 +4412,7 @@
         <v>282</v>
       </c>
       <c r="B281">
-        <v>17812.560000000001</v>
+        <v>19304.351999999999</v>
       </c>
       <c r="C281">
         <v>0</v>
@@ -4414,7 +4423,7 @@
         <v>283</v>
       </c>
       <c r="B282">
-        <v>17889.094000000001</v>
+        <v>19398.343000000001</v>
       </c>
       <c r="C282">
         <v>0</v>
@@ -4425,7 +4434,7 @@
         <v>284</v>
       </c>
       <c r="B283">
-        <v>17979.218000000001</v>
+        <v>19506.949000000001</v>
       </c>
       <c r="C283">
         <v>0</v>
@@ -4436,7 +4445,7 @@
         <v>285</v>
       </c>
       <c r="B284">
-        <v>18127.993999999999</v>
+        <v>19660.766</v>
       </c>
       <c r="C284">
         <v>0</v>
@@ -4447,7 +4456,7 @@
         <v>286</v>
       </c>
       <c r="B285">
-        <v>18310.3</v>
+        <v>19882.351999999999</v>
       </c>
       <c r="C285">
         <v>0</v>
@@ -4458,7 +4467,7 @@
         <v>287</v>
       </c>
       <c r="B286">
-        <v>18437.127</v>
+        <v>20044.077000000001</v>
       </c>
       <c r="C286">
         <v>0</v>
@@ -4469,7 +4478,7 @@
         <v>288</v>
       </c>
       <c r="B287">
-        <v>18565.697</v>
+        <v>20150.475999999999</v>
       </c>
       <c r="C287">
         <v>0</v>
@@ -4480,7 +4489,7 @@
         <v>289</v>
       </c>
       <c r="B288">
-        <v>18699.748</v>
+        <v>20276.153999999999</v>
       </c>
       <c r="C288">
         <v>0</v>
@@ -4491,7 +4500,7 @@
         <v>290</v>
       </c>
       <c r="B289">
-        <v>18733.741000000002</v>
+        <v>20304.874</v>
       </c>
       <c r="C289">
         <v>0</v>
@@ -4502,7 +4511,7 @@
         <v>291</v>
       </c>
       <c r="B290">
-        <v>18835.411</v>
+        <v>20415.150000000001</v>
       </c>
       <c r="C290">
         <v>0</v>
@@ -4513,7 +4522,7 @@
         <v>292</v>
       </c>
       <c r="B291">
-        <v>18962.174999999999</v>
+        <v>20584.527999999998</v>
       </c>
       <c r="C291">
         <v>0</v>
@@ -4524,7 +4533,7 @@
         <v>293</v>
       </c>
       <c r="B292">
-        <v>19130.932000000001</v>
+        <v>20817.580999999998</v>
       </c>
       <c r="C292">
         <v>0</v>
@@ -4535,7 +4544,7 @@
         <v>294</v>
       </c>
       <c r="B293">
-        <v>19215.690999999999</v>
+        <v>20951.088</v>
       </c>
       <c r="C293">
         <v>0</v>
@@ -4546,7 +4555,7 @@
         <v>295</v>
       </c>
       <c r="B294">
-        <v>18989.877</v>
+        <v>20665.553</v>
       </c>
       <c r="C294">
         <v>1</v>
@@ -4557,7 +4566,7 @@
         <v>296</v>
       </c>
       <c r="B295">
-        <v>17378.712</v>
+        <v>19034.830000000002</v>
       </c>
       <c r="C295">
         <v>1</v>
@@ -4568,7 +4577,7 @@
         <v>297</v>
       </c>
       <c r="B296">
-        <v>18743.72</v>
+        <v>20511.785</v>
       </c>
       <c r="C296">
         <v>0</v>
@@ -4579,7 +4588,7 @@
         <v>298</v>
       </c>
       <c r="B297">
-        <v>18924.261999999999</v>
+        <v>20724.128000000001</v>
       </c>
       <c r="C297">
         <v>0</v>
@@ -4590,7 +4599,7 @@
         <v>299</v>
       </c>
       <c r="B298">
-        <v>19216.223999999998</v>
+        <v>20990.541000000001</v>
       </c>
       <c r="C298">
         <v>0</v>
@@ -4601,7 +4610,7 @@
         <v>300</v>
       </c>
       <c r="B299">
-        <v>19544.248</v>
+        <v>21309.544000000002</v>
       </c>
       <c r="C299">
         <v>0</v>
@@ -4612,7 +4621,7 @@
         <v>301</v>
       </c>
       <c r="B300">
-        <v>19672.594000000001</v>
+        <v>21483.082999999999</v>
       </c>
       <c r="C300">
         <v>0</v>
@@ -4623,7 +4632,7 @@
         <v>302</v>
       </c>
       <c r="B301">
-        <v>20006.181</v>
+        <v>21847.601999999999</v>
       </c>
       <c r="C301">
         <v>0</v>
@@ -4634,7 +4643,7 @@
         <v>303</v>
       </c>
       <c r="B302">
-        <v>19924.088</v>
+        <v>21738.870999999999</v>
       </c>
       <c r="C302">
         <v>0</v>
@@ -4645,7 +4654,7 @@
         <v>304</v>
       </c>
       <c r="B303">
-        <v>19895.271000000001</v>
+        <v>21708.16</v>
       </c>
       <c r="C303">
         <v>0</v>
@@ -4656,7 +4665,7 @@
         <v>305</v>
       </c>
       <c r="B304">
-        <v>20054.663</v>
+        <v>21851.133999999998</v>
       </c>
       <c r="C304">
         <v>0</v>
@@ -4667,7 +4676,7 @@
         <v>306</v>
       </c>
       <c r="B305">
-        <v>20182.491000000002</v>
+        <v>21989.981</v>
       </c>
       <c r="C305">
         <v>0</v>
@@ -4677,7 +4686,43 @@
       <c r="A306" s="1" t="s">
         <v>307</v>
       </c>
+      <c r="B306">
+        <v>22112.329000000002</v>
+      </c>
       <c r="C306">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A307" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B307">
+        <v>22225.35</v>
+      </c>
+      <c r="C307">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A308" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B308">
+        <v>22490.691999999999</v>
+      </c>
+      <c r="C308">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A309" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B309">
+        <v>22679.255000000001</v>
+      </c>
+      <c r="C309">
         <v>0</v>
       </c>
     </row>

</xml_diff>